<commit_message>
a ton of database work
</commit_message>
<xml_diff>
--- a/data/extracted_data/raw_round1/timeseries/Barbosa_etal_2019_Fig1.xlsx
+++ b/data/extracted_data/raw_round1/timeseries/Barbosa_etal_2019_Fig1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/hab_depuration/data/extracted_data/raw/timeseries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/hab_depuration/data/extracted_data/raw_round1/timeseries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549CA41C-E6D2-B543-979A-875E998FAEA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1B4BA2-09F7-7842-AD2A-09721D82C5B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8540" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{80B0784C-6CFF-E44D-A606-AD56627BBE0D}"/>
+    <workbookView xWindow="8540" yWindow="500" windowWidth="34660" windowHeight="24260" xr2:uid="{80B0784C-6CFF-E44D-A606-AD56627BBE0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="19">
   <si>
     <t>treatment</t>
   </si>
@@ -97,6 +86,12 @@
   </si>
   <si>
     <t>24°C</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Derived</t>
   </si>
 </sst>
 </file>
@@ -480,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A4A5A2-7E85-7340-B756-77DB99BA5698}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1057,7 +1052,184 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="C29" s="1"/>
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>0.28122994652406441</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>0.52748663101604198</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>0.58030748663101472</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>0.49129679144385013</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>0.54340909090909018</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>1.6365775401069516</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35">
+        <v>6</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36">
+        <v>6</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37">
+        <v>6</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>